<commit_message>
Revision de funcionalidades de responsive
</commit_message>
<xml_diff>
--- a/Seguimiento-Consignas/Entrega-Final-Cumplimiento-Consignas.xlsx
+++ b/Seguimiento-Consignas/Entrega-Final-Cumplimiento-Consignas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cusro-CodoACodo\06-JS-FrontEnd-24225\C24225SLC-FINAL\Seguimiento-Consignas\Entrega-Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cusro-CodoACodo\06-JS-FrontEnd-24225\C24225SLC\Seguimiento-Consignas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C8B682-A65F-457E-A1A8-D1CAB247BA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B512B28-AABF-4CF6-A9F1-1C45EEBB1ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{E73603EF-647A-4F8D-8F20-EFE93E8FD641}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="69">
   <si>
     <t>Consigna</t>
   </si>
@@ -63,13 +63,7 @@
     <t>Inclusión de un archivo README.md que explique brevemente el propósito de la página.</t>
   </si>
   <si>
-    <t>Se incluye readme.md. Puede encontrarse en el repositorio GIT:</t>
-  </si>
-  <si>
     <t>Creación de un formulario de contacto con campos de nombre, correo electrónico y mensaje, utilizando Formspree.</t>
-  </si>
-  <si>
-    <t>Puede encontrarse en static/contacto.html</t>
   </si>
   <si>
     <t>Deberás incluir archivos multimedia (imagenes e iframes) funcionales al contenido de la página.</t>
@@ -89,11 +83,6 @@
     <t>El proyecto debe estar subido a un hosting gratuito (Netlify o GitHub Pages), con una URL funcional.</t>
   </si>
   <si>
-    <t>Para netifly: https://sportsprook.netlify.app/ 
-Para github: https://contesl.github.io/C24225SLC/C24225SLC.git
-Para github page: https://github.com/contesl/</t>
-  </si>
-  <si>
     <t>Estructura semántica: El HTML debe estar dividido en las etiquetas semánticas principales: header, nav, main, section, footer</t>
   </si>
   <si>
@@ -116,9 +105,6 @@
     <t xml:space="preserve">Sección "Contacto": Debe ser responsiva mediante el uso de Media Queries para adaptarse a diferentes tamaños de pantalla. </t>
   </si>
   <si>
-    <t>Se implementa en la pagina static/contacto.html</t>
-  </si>
-  <si>
     <t>Estructura basica HTML</t>
   </si>
   <si>
@@ -156,9 +142,6 @@
   </si>
   <si>
     <t>Implementar las propiedades de Box Modeling (márgenes, rellenos, bordes) en los diferentes elementos del proyecto.</t>
-  </si>
-  <si>
-    <t>Se implementa en las diferentes paginas a traves de los estilos existentes en css/style.css</t>
   </si>
   <si>
     <t>Uso de Bootstrap y Git</t>
@@ -171,9 +154,6 @@
     <t>El proyecto debe estar en un repositorio GitHub, con commits que documenten los cambios.</t>
   </si>
   <si>
-    <t>Para github: https://contesl.github.io/C24225SLC/C24225SLC.git</t>
-  </si>
-  <si>
     <t>Funcionalidad JavaScript</t>
   </si>
   <si>
@@ -229,17 +209,7 @@
     <t>La validacion del formulario de contacto se encuenta en js/validarContacto.js</t>
   </si>
   <si>
-    <t>Se implemeta el menu de navegacion de Bootstrap.</t>
-  </si>
-  <si>
     <t>Se puede revisar el codigo sin problemas con las herramientas de desarrollador de Chrome</t>
-  </si>
-  <si>
-    <t>Esto puede encontrarse en js/productos.js</t>
-  </si>
-  <si>
-    <t>Se utiliza un script para validacion de formulario de contacto: js/validarContacto.js
-Se utiliza un script para armado dinamico de pagina de productos: js/productos.js</t>
   </si>
   <si>
     <t>Esto puede encontrarse en js/productos.js
@@ -248,6 +218,48 @@
   </si>
   <si>
     <t>Toda la operatoria puede encontrarse en static/productos.html y js/productos.js</t>
+  </si>
+  <si>
+    <t>Se incluye readme.md. Puede encontrarse en el repositorio GIT</t>
+  </si>
+  <si>
+    <t>Para netifly: https://sportsprook.netlify.app/ 
+Para repositorio github:  https://github.com/contesl/</t>
+  </si>
+  <si>
+    <t>Puede encontrarse en static/contacto.html
+Cuando se genera el contacto Formspree devuelve el mensaje de recepcion y envia un email a la cuenta registrada</t>
+  </si>
+  <si>
+    <t>Se implementa en la pagina static/contacto.html
+El soporte a multiples formatos esta implementado en css/styles.css</t>
+  </si>
+  <si>
+    <t>Se implementa en todas las paginas desde los los estilos existentes en css/style.css</t>
+  </si>
+  <si>
+    <t>Se implemeta el menu de navegacion de Bootstrap.
+Revisar cada pagina para ver la implementacion</t>
+  </si>
+  <si>
+    <t>Para repositorio github:  https://github.com/contesl/</t>
+  </si>
+  <si>
+    <t>Revisar el directorio js para encontrar los scrips que se utilizan en las paginas que asi lo requieren:
+productos.js : para el armado dinamico de la pagina de productos luego de un fetch a una api publicada sumado al tratamiento del carrito de compra
+resenials.js: para el armado de las reseñas de productos a partir del fetch de la api utilizada en productos.js que tambien contiene las reseñas
+validarContacto.js: validacion de datos del formulario de contacto</t>
+  </si>
+  <si>
+    <t>Esto puede encontrarse en js/productos.js
+En la pagina productos.html, cuando se posiciona del cursor en la imagen de un producto, cambia el formato del cursor y se puede acceder a su descripcion ampliada</t>
+  </si>
+  <si>
+    <t>Esto puede encontrarse en js/productos.js
+esto se puede encontrar buscando el comentario   // Cargar el JSON desde el archivo local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esto puede encontrarse en js/productos.js y  en js/resenias.js porque se utilizo la misma api publica dado que contienen los datos requeridos </t>
   </si>
 </sst>
 </file>
@@ -401,9 +413,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -421,6 +430,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -759,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD66D113-014E-4A55-AA96-4F35F8EF79FF}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,16 +806,16 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="23"/>
+      <c r="C3" s="22"/>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>3</v>
@@ -820,83 +832,83 @@
         <v>3</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="23"/>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C6" s="22"/>
+    </row>
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>10</v>
+      <c r="C7" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="24"/>
+      <c r="C8" s="23"/>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="23"/>
-    </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="C11" s="22"/>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>1</v>
@@ -905,291 +917,291 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="25"/>
+      <c r="C17" s="24"/>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="21" t="s">
-        <v>24</v>
+      <c r="C20" s="17" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="25"/>
+      <c r="C21" s="24"/>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="26"/>
+      <c r="C23" s="25"/>
     </row>
     <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="22" t="s">
-        <v>61</v>
+      <c r="C24" s="28" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="26"/>
-    </row>
-    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
-        <v>44</v>
+      <c r="C26" s="25"/>
+    </row>
+    <row r="27" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>38</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B29" s="15"/>
-      <c r="C29" s="26"/>
+      <c r="C29" s="25"/>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="22" t="s">
-        <v>60</v>
+      <c r="C30" s="21" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="28" t="s">
-        <v>48</v>
+      <c r="A31" s="27" t="s">
+        <v>42</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B32" s="15"/>
-      <c r="C32" s="26"/>
-    </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C32" s="25"/>
+    </row>
+    <row r="33" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="22" t="s">
-        <v>63</v>
+      <c r="C33" s="28" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
-        <v>51</v>
+      <c r="A34" s="27" t="s">
+        <v>45</v>
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="26"/>
+      <c r="C35" s="25"/>
     </row>
     <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="22" t="s">
-        <v>63</v>
+      <c r="C36" s="28" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="26"/>
+      <c r="C37" s="25"/>
     </row>
     <row r="38" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>55</v>
+      <c r="A38" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="18" t="s">
+      <c r="C38" s="26" t="s">
         <v>56</v>
       </c>
+    </row>
+    <row r="39" spans="1:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
+        <v>50</v>
+      </c>
       <c r="B39" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C39" s="22" t="s">
-        <v>63</v>
+      <c r="C39" s="17" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="26"/>
+      <c r="C40" s="25"/>
     </row>
     <row r="41" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="22" t="s">
-        <v>66</v>
+      <c r="C42" s="21" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>